<commit_message>
Saioan insert gehiago sartu ditut
</commit_message>
<xml_diff>
--- a/SQL/Zinema/ZinemaInsert.xlsx
+++ b/SQL/Zinema/ZinemaInsert.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\in1dm3-d\Desktop\db\erronka3\SQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\in1dm3-d\Desktop\db\erronka3\SQL\Zinema\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>